<commit_message>
Added patient data, Uen, fasting BG.
</commit_message>
<xml_diff>
--- a/1. Detemir/My Code/Data/patient_master.xlsx
+++ b/1. Detemir/My Code/Data/patient_master.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22524"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Glycaemic Control FYP 2018 - Klenner\2 - Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1588\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_1496B87DFFF4802DA455672374E7D0BBBE616D69" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pt1" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,18 @@
     <sheet name="pt4" sheetId="4" r:id="rId4"/>
     <sheet name="pt5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -168,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -354,7 +363,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -792,7 +800,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1230,7 +1237,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3344,7 +3350,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3374,7 +3386,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3404,7 +3422,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3684,7 +3708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4490,7 +4514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4864,7 +4888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5659,7 +5683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6433,7 +6457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>